<commit_message>
rows reference gen code updated.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,12 +8,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>
-            32
-        </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>
             Hello
@@ -31,19 +26,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="n">
+        <v>
+                    32
+                </v>
+      </c>
+      <c r="B1" t="s">
         <v>
                     0
                 </v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>
+                        This string is embeded
+                    </t>
+        </is>
+      </c>
+      <c r="Z1" t="s">
         <v>
                     1
                 </v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="n">
         <v>
-                    2
+                    53
                 </v>
       </c>
     </row>

</xml_diff>